<commit_message>
updated version instr var est data
</commit_message>
<xml_diff>
--- a/Paper1/Data/instrumental_variable_est.xlsx
+++ b/Paper1/Data/instrumental_variable_est.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basmachielsen/Documents/git/UU_PhD_BasMachielsen/Paper1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDEE403-3395-3749-BD69-79CBE14FE6BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC737848-10A1-4B4E-85D4-162A18B9D38A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{1978E0BF-9847-6B4D-B01E-44B742104530}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{1978E0BF-9847-6B4D-B01E-44B742104530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{DD37B853-59D8-284E-B51B-F091A3EC8B83}" name="instrumental_variable_wealth_par" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/basmachielsen/Documents/git/UU_PhD_BasMachielsen/Paper1/Data/instrumental_variable_wealth_par.csv" decimal="," thousands="." semicolon="1">
+    <textPr sourceFile="/Users/basmachielsen/Documents/git/UU_PhD_BasMachielsen/Paper1/Data/instrumental_variable_wealth_par.csv" decimal="," thousands="." semicolon="1">
       <textFields count="11">
         <textField type="text"/>
         <textField type="text"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="1111">
   <si>
     <t>polid</t>
   </si>
@@ -3203,6 +3203,192 @@
   </si>
   <si>
     <t>1832-08-06</t>
+  </si>
+  <si>
+    <t>1853-04-04</t>
+  </si>
+  <si>
+    <t>https://nl.wikipedia.org/wiki/Jan_Willem_Conrad</t>
+  </si>
+  <si>
+    <t>Zwolle</t>
+  </si>
+  <si>
+    <t>1883-05-13</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Juliana-Louisa-Lenssen/6000000017051917800</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>1855-07-25</t>
+  </si>
+  <si>
+    <t>https://nl.wikipedia.org/wiki/Jan_Corver_Hooft</t>
+  </si>
+  <si>
+    <t>s-Graveland</t>
+  </si>
+  <si>
+    <t>1837-12-03</t>
+  </si>
+  <si>
+    <t>https://www.genealogieonline.nl/stamboom-tolsma/I39447.php</t>
+  </si>
+  <si>
+    <t>1869-06-20</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Jacob-Theodoor-Cremer/6000000016289378610</t>
+  </si>
+  <si>
+    <t>1874-12-10</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Louise-Water/6000000016289416424</t>
+  </si>
+  <si>
+    <t>1845-07-30</t>
+  </si>
+  <si>
+    <t>https://nl.wikipedia.org/wiki/Franciscus_Jacobus_Joannes_Cremers</t>
+  </si>
+  <si>
+    <t>1842-04-12</t>
+  </si>
+  <si>
+    <t>https://www.openarch.nl/gra:5ee990f1-7411-cf39-8b33-319846932de3</t>
+  </si>
+  <si>
+    <t>1866-05-28</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Godert-Willem-van-Dedem-van-den-Berg-baron/6000000016794079360</t>
+  </si>
+  <si>
+    <t>Dalfsen</t>
+  </si>
+  <si>
+    <t>1843-02-02</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Grietjen-Boxem/6000000016794130165</t>
+  </si>
+  <si>
+    <t>1858-08-07</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Steven-van-Delden/6000000017955695351</t>
+  </si>
+  <si>
+    <t>Winterswijk?</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Engelina-Elisabeth-Schutte/6000000017955695357</t>
+  </si>
+  <si>
+    <t>https://www.openarch.nl/hga:E8D6E7AD-C584-44F2-84F1-C63267B0B2E9</t>
+  </si>
+  <si>
+    <t>1910-12-25</t>
+  </si>
+  <si>
+    <t>1892-05-14</t>
+  </si>
+  <si>
+    <t>http://www.biografischportaal.nl/persoon/99433997</t>
+  </si>
+  <si>
+    <t>Dordrecht</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Maria-Elisabeth-Allegonda-Soiron/6000000028892163968</t>
+  </si>
+  <si>
+    <t>Nijmegen</t>
+  </si>
+  <si>
+    <t>1886-11-27</t>
+  </si>
+  <si>
+    <t>1880-02-29</t>
+  </si>
+  <si>
+    <t>https://gw.geneanet.org/assel209?lang=en&amp;pz=joannes&amp;nz=asselberghs&amp;p=johann+peter&amp;n=dobbelmann</t>
+  </si>
+  <si>
+    <t>1885-06-25</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Jakob-Dolk/6000000023794685073</t>
+  </si>
+  <si>
+    <t>Etten-Leur?</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Wilhelmina-van-der-Burgt/6000000023794419298</t>
+  </si>
+  <si>
+    <t>1881-08-01</t>
+  </si>
+  <si>
+    <t>1839-08-14</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Johannes-Donner/6000000026587193211</t>
+  </si>
+  <si>
+    <t>1863-08-19</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Aleijda-Koopman/6000000026587281268</t>
+  </si>
+  <si>
+    <t>1882-08-02</t>
+  </si>
+  <si>
+    <t>https://nl.wikipedia.org/wiki/Elisa_Cornelis_Unico_van_Doorn</t>
+  </si>
+  <si>
+    <t>Maarn</t>
+  </si>
+  <si>
+    <t>https://www.geni.com/people/Rudolphine-Weerts/6000000017477968730</t>
+  </si>
+  <si>
+    <t>1895</t>
+  </si>
+  <si>
+    <t>Velp, Rheden</t>
+  </si>
+  <si>
+    <t>https://www.genealogieonline.nl/stamboom_drion/I9.php</t>
+  </si>
+  <si>
+    <t>1886-11-06</t>
+  </si>
+  <si>
+    <t>https://www.genealogieonline.nl/stamboom_drion/I13.php</t>
+  </si>
+  <si>
+    <t>1937-09-08</t>
+  </si>
+  <si>
+    <t>Putten</t>
+  </si>
+  <si>
+    <t>http://www.jodeninnederland.nl/id/P-3871</t>
+  </si>
+  <si>
+    <t>Voorschoten</t>
+  </si>
+  <si>
+    <t>https://www.openarch.nl/search.php?name=Johanna+Carolina+Christina+Margaretha+Therese+Temme</t>
+  </si>
+  <si>
+    <t>1884-04-08</t>
   </si>
 </sst>
 </file>
@@ -3247,10 +3433,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3572,8 +3759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCA590D-D655-0D41-8189-7502BFDA6186}">
   <dimension ref="A1:M265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4678,7 +4865,24 @@
       <c r="E45" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="J45" t="s">
+        <v>1053</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>1054</v>
+      </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
@@ -4696,7 +4900,21 @@
       <c r="E46" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J46" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
@@ -4714,7 +4932,24 @@
       <c r="E47" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J47" t="s">
+        <v>1063</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
@@ -4732,9 +4967,26 @@
       <c r="E48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="F48" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="J48" t="s">
+        <v>1067</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
         <v>446</v>
       </c>
@@ -4752,16 +5004,33 @@
       </c>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
         <v>448</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="F50" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G50" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="J50" t="s">
+        <v>1072</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
         <v>89</v>
       </c>
@@ -4776,7 +5045,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:11">
       <c r="A52" s="1" t="s">
         <v>451</v>
       </c>
@@ -4792,9 +5061,23 @@
       <c r="E52" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="F52" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J52" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="1" t="s">
         <v>453</v>
       </c>
@@ -4810,9 +5093,23 @@
       <c r="E53" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="F53" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J53" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
         <v>456</v>
       </c>
@@ -4828,8 +5125,26 @@
       <c r="E54" s="1" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="F54" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J54" t="s">
+        <v>1082</v>
+      </c>
+      <c r="K54" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
         <v>459</v>
       </c>
@@ -4845,8 +5160,26 @@
       <c r="E55" s="1" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="F55" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G55" t="s">
+        <v>1088</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J55" t="s">
+        <v>1090</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
         <v>462</v>
       </c>
@@ -4862,8 +5195,26 @@
       <c r="E56" s="1" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="F56" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G56" t="s">
+        <v>1093</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J56" t="s">
+        <v>1095</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="1" t="s">
         <v>465</v>
       </c>
@@ -4879,8 +5230,26 @@
       <c r="E57" s="1" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="F57" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G57" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="J57" t="s">
+        <v>1099</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="1" t="s">
         <v>469</v>
       </c>
@@ -4896,8 +5265,26 @@
       <c r="E58" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="F58" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1102</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="J58" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="1" t="s">
         <v>472</v>
       </c>
@@ -4913,8 +5300,20 @@
       <c r="E59" s="1" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="F59" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J59" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="1" t="s">
         <v>475</v>
       </c>
@@ -4931,7 +5330,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:11">
       <c r="A61" s="1" t="s">
         <v>477</v>
       </c>
@@ -4948,7 +5347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:11">
       <c r="A62" s="1" t="s">
         <v>479</v>
       </c>
@@ -4965,7 +5364,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
         <v>479</v>
       </c>
@@ -4982,7 +5381,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:11">
       <c r="A64" s="1" t="s">
         <v>482</v>
       </c>

</xml_diff>

<commit_message>
add wealth correction code
</commit_message>
<xml_diff>
--- a/Paper1/Data/instrumental_variable_est.xlsx
+++ b/Paper1/Data/instrumental_variable_est.xlsx
@@ -4772,11 +4772,11 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F183" activeCellId="0" sqref="F183"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.33"/>

</xml_diff>